<commit_message>
Regretion Run SCD0044 - Filter Lead Kelolaan, SCD0045 - Filter Lead Prospek, SCD0046 - Filter Pipeline Monitoring, SCD0047 - Filter Pipeline Closing, SCD0048_Filter Pipeline Follow Up, SCD0049_Filter Pipeline Cart, and SCD0050- Account Plan - Usulan
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0045_Filter Lead Prospek.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0045_Filter Lead Prospek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1136D5-09A8-46C2-8141-C52D58CFDA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A33A63-B6F4-4C38-A46B-9D7AB2AC5342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="2925" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0045" sheetId="2" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>Inquiry &amp; filtering Data Lead Prospek</t>
   </si>
   <si>
-    <t>Azara</t>
+    <t>ya</t>
   </si>
 </sst>
 </file>

</xml_diff>